<commit_message>
findings in test-suite Fixes #210
</commit_message>
<xml_diff>
--- a/testing/AdministratorAdministration+testcase.docs.xlsx
+++ b/testing/AdministratorAdministration+testcase.docs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IS00759329\Desktop\Telefonica\ApplicationPattern\ApplicationPattern_v2\AdministratorAdministration\AdministratorAdministration-5\testing\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F9D39394-540D-461A-AE25-2F05CE155229}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3C956DED-3879-4D89-AA50-BECB177B8DDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8A4BF7CC-909B-4C1B-B59F-29AF2D960B3A}"/>
+    <workbookView xWindow="285" yWindow="270" windowWidth="20205" windowHeight="10650" xr2:uid="{8A4BF7CC-909B-4C1B-B59F-29AF2D960B3A}"/>
   </bookViews>
   <sheets>
     <sheet name="Servicelayer" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="497" uniqueCount="228">
   <si>
     <t>Testcases</t>
   </si>
@@ -1382,6 +1382,14 @@
   - dummy values generated for application-name, release-number, address, protocol, port 
    -operation-key from above
    - reasonable parameter</t>
+  </si>
+  <si>
+    <t>#### Clearing:
+- PUT initial newRelease/application-name
+- PUT initial newRelease/release-number
+- PUT initial newRelease/protocol
+- PUT initial newRelease/address
+- PUT initial newRelease/port</t>
   </si>
 </sst>
 </file>
@@ -1830,9 +1838,6 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1840,16 +1845,19 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2171,15 +2179,15 @@
   <dimension ref="A1:G239"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="3" topLeftCell="B133" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="G139" sqref="G139"/>
+      <selection pane="bottomRight" activeCell="C135" sqref="C135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="35.5703125" style="61" customWidth="1"/>
+    <col min="1" max="1" width="35.5703125" style="58" customWidth="1"/>
     <col min="2" max="2" width="70.7109375" style="2"/>
     <col min="3" max="6" width="70.7109375" style="52"/>
     <col min="7" max="7" width="70.7109375" style="52" customWidth="1"/>
@@ -2234,7 +2242,7 @@
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="55" t="s">
+      <c r="A4" s="59" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="4" t="s">
@@ -2262,7 +2270,7 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="225" x14ac:dyDescent="0.25">
-      <c r="A5" s="55"/>
+      <c r="A5" s="59"/>
       <c r="B5" s="5" t="s">
         <v>5</v>
       </c>
@@ -2345,7 +2353,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="55"/>
+      <c r="A6" s="59"/>
       <c r="B6" s="5" t="s">
         <v>6</v>
       </c>
@@ -2379,7 +2387,7 @@
       </c>
     </row>
     <row r="7" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="55"/>
+      <c r="A7" s="59"/>
       <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
@@ -2408,7 +2416,7 @@
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" s="55" t="s">
+      <c r="A8" s="59" t="s">
         <v>8</v>
       </c>
       <c r="B8" s="7" t="s">
@@ -2436,7 +2444,7 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="255" x14ac:dyDescent="0.25">
-      <c r="A9" s="55"/>
+      <c r="A9" s="59"/>
       <c r="B9" s="8" t="s">
         <v>10</v>
       </c>
@@ -2518,7 +2526,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="55"/>
+      <c r="A10" s="59"/>
       <c r="B10" s="8" t="s">
         <v>11</v>
       </c>
@@ -2549,7 +2557,7 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A11" s="55"/>
+      <c r="A11" s="59"/>
       <c r="B11" s="6" t="str">
         <f>$B7</f>
         <v>#### Clearing:
@@ -2580,7 +2588,7 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="55" t="s">
+      <c r="A12" s="59" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="7" t="s">
@@ -2608,7 +2616,7 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="255" x14ac:dyDescent="0.25">
-      <c r="A13" s="55"/>
+      <c r="A13" s="59"/>
       <c r="B13" s="8" t="s">
         <v>14</v>
       </c>
@@ -2692,7 +2700,7 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="55"/>
+      <c r="A14" s="59"/>
       <c r="B14" s="8" t="s">
         <v>15</v>
       </c>
@@ -2723,7 +2731,7 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A15" s="55"/>
+      <c r="A15" s="59"/>
       <c r="B15" s="6" t="str">
         <f>$B7</f>
         <v>#### Clearing:
@@ -2754,7 +2762,7 @@
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" s="55" t="s">
+      <c r="A16" s="59" t="s">
         <v>16</v>
       </c>
       <c r="B16" s="7" t="s">
@@ -2782,7 +2790,7 @@
       </c>
     </row>
     <row r="17" spans="1:7" ht="240" x14ac:dyDescent="0.25">
-      <c r="A17" s="55"/>
+      <c r="A17" s="59"/>
       <c r="B17" s="8" t="s">
         <v>18</v>
       </c>
@@ -2863,7 +2871,7 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="55"/>
+      <c r="A18" s="59"/>
       <c r="B18" s="8" t="s">
         <v>15</v>
       </c>
@@ -2894,7 +2902,7 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A19" s="55"/>
+      <c r="A19" s="59"/>
       <c r="B19" s="6" t="str">
         <f>$B7</f>
         <v>#### Clearing:
@@ -2925,7 +2933,7 @@
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="55" t="s">
+      <c r="A20" s="59" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="7" t="s">
@@ -2953,7 +2961,7 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="240" x14ac:dyDescent="0.25">
-      <c r="A21" s="55"/>
+      <c r="A21" s="59"/>
       <c r="B21" s="8" t="s">
         <v>21</v>
       </c>
@@ -3034,7 +3042,7 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="55"/>
+      <c r="A22" s="59"/>
       <c r="B22" s="8" t="s">
         <v>15</v>
       </c>
@@ -3065,7 +3073,7 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A23" s="55"/>
+      <c r="A23" s="59"/>
       <c r="B23" s="6" t="str">
         <f>$B7</f>
         <v>#### Clearing:
@@ -3096,7 +3104,7 @@
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="55" t="s">
+      <c r="A24" s="59" t="s">
         <v>22</v>
       </c>
       <c r="B24" s="7" t="s">
@@ -3124,7 +3132,7 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="210" x14ac:dyDescent="0.25">
-      <c r="A25" s="55"/>
+      <c r="A25" s="59"/>
       <c r="B25" s="8" t="s">
         <v>24</v>
       </c>
@@ -3195,7 +3203,7 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="55"/>
+      <c r="A26" s="59"/>
       <c r="B26" s="8" t="s">
         <v>25</v>
       </c>
@@ -3226,7 +3234,7 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A27" s="55"/>
+      <c r="A27" s="59"/>
       <c r="B27" s="6" t="str">
         <f>$B7</f>
         <v>#### Clearing:
@@ -3257,7 +3265,7 @@
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A28" s="55" t="s">
+      <c r="A28" s="59" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="7" t="s">
@@ -3285,7 +3293,7 @@
       </c>
     </row>
     <row r="29" spans="1:7" ht="210" x14ac:dyDescent="0.25">
-      <c r="A29" s="55"/>
+      <c r="A29" s="59"/>
       <c r="B29" s="8" t="s">
         <v>28</v>
       </c>
@@ -3356,7 +3364,7 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="55"/>
+      <c r="A30" s="59"/>
       <c r="B30" s="8" t="s">
         <v>25</v>
       </c>
@@ -3387,7 +3395,7 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A31" s="55"/>
+      <c r="A31" s="59"/>
       <c r="B31" s="6" t="str">
         <f>$B7</f>
         <v>#### Clearing:
@@ -3418,7 +3426,7 @@
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="55" t="s">
+      <c r="A32" s="59" t="s">
         <v>29</v>
       </c>
       <c r="B32" s="7" t="s">
@@ -3446,7 +3454,7 @@
       </c>
     </row>
     <row r="33" spans="1:7" ht="225" x14ac:dyDescent="0.25">
-      <c r="A33" s="55"/>
+      <c r="A33" s="59"/>
       <c r="B33" s="8" t="s">
         <v>31</v>
       </c>
@@ -3506,7 +3514,7 @@
       </c>
     </row>
     <row r="34" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A34" s="55"/>
+      <c r="A34" s="59"/>
       <c r="B34" s="8" t="s">
         <v>32</v>
       </c>
@@ -3533,7 +3541,7 @@
       </c>
     </row>
     <row r="35" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A35" s="55"/>
+      <c r="A35" s="59"/>
       <c r="B35" s="6" t="str">
         <f>$B7</f>
         <v>#### Clearing:
@@ -3564,7 +3572,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="55" t="s">
+      <c r="A36" s="59" t="s">
         <v>33</v>
       </c>
       <c r="B36" s="7" t="s">
@@ -3592,7 +3600,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" ht="225" x14ac:dyDescent="0.25">
-      <c r="A37" s="55"/>
+      <c r="A37" s="59"/>
       <c r="B37" s="8" t="s">
         <v>31</v>
       </c>
@@ -3652,7 +3660,7 @@
       </c>
     </row>
     <row r="38" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A38" s="55"/>
+      <c r="A38" s="59"/>
       <c r="B38" s="8" t="s">
         <v>35</v>
       </c>
@@ -3682,7 +3690,7 @@
       </c>
     </row>
     <row r="39" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A39" s="55"/>
+      <c r="A39" s="59"/>
       <c r="B39" s="6" t="str">
         <f>$B7</f>
         <v>#### Clearing:
@@ -3713,7 +3721,7 @@
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A40" s="55" t="s">
+      <c r="A40" s="59" t="s">
         <v>36</v>
       </c>
       <c r="B40" s="7" t="s">
@@ -3741,7 +3749,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" ht="225" x14ac:dyDescent="0.25">
-      <c r="A41" s="56"/>
+      <c r="A41" s="60"/>
       <c r="B41" s="8" t="s">
         <v>31</v>
       </c>
@@ -3801,7 +3809,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A42" s="56"/>
+      <c r="A42" s="60"/>
       <c r="B42" s="8" t="s">
         <v>38</v>
       </c>
@@ -3847,7 +3855,7 @@
       </c>
     </row>
     <row r="43" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A43" s="56"/>
+      <c r="A43" s="60"/>
       <c r="B43" s="6" t="str">
         <f>$B7</f>
         <v>#### Clearing:
@@ -3878,7 +3886,7 @@
       </c>
     </row>
     <row r="44" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A44" s="55" t="s">
+      <c r="A44" s="59" t="s">
         <v>39</v>
       </c>
       <c r="B44" s="7" t="s">
@@ -3901,7 +3909,7 @@
       </c>
     </row>
     <row r="45" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="56"/>
+      <c r="A45" s="60"/>
       <c r="B45" s="8" t="s">
         <v>41</v>
       </c>
@@ -3922,7 +3930,7 @@
       </c>
     </row>
     <row r="46" spans="1:7" ht="300" x14ac:dyDescent="0.25">
-      <c r="A46" s="56"/>
+      <c r="A46" s="60"/>
       <c r="B46" s="8" t="s">
         <v>205</v>
       </c>
@@ -4038,7 +4046,7 @@
       </c>
     </row>
     <row r="47" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A47" s="56"/>
+      <c r="A47" s="60"/>
       <c r="B47" s="8" t="s">
         <v>206</v>
       </c>
@@ -4124,7 +4132,7 @@
       </c>
     </row>
     <row r="48" spans="1:7" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="56"/>
+      <c r="A48" s="60"/>
       <c r="B48" s="9" t="str">
         <f>$B7</f>
         <v>#### Clearing:
@@ -4155,7 +4163,7 @@
       </c>
     </row>
     <row r="49" spans="1:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="57" t="s">
+      <c r="A49" s="56" t="s">
         <v>42</v>
       </c>
       <c r="B49" s="10"/>
@@ -4166,7 +4174,7 @@
       <c r="G49" s="3"/>
     </row>
     <row r="50" spans="1:7" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="58" t="s">
+      <c r="A50" s="61" t="s">
         <v>43</v>
       </c>
       <c r="B50" s="11" t="s">
@@ -4188,8 +4196,8 @@
         <v>129</v>
       </c>
     </row>
-    <row r="51" spans="1:7" ht="180" x14ac:dyDescent="0.25">
-      <c r="A51" s="55"/>
+    <row r="51" spans="1:7" ht="150" x14ac:dyDescent="0.25">
+      <c r="A51" s="59"/>
       <c r="B51" s="12" t="s">
         <v>45</v>
       </c>
@@ -4230,7 +4238,7 @@
       </c>
     </row>
     <row r="52" spans="1:7" ht="171" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="55"/>
+      <c r="A52" s="59"/>
       <c r="B52" s="13" t="s">
         <v>46</v>
       </c>
@@ -4251,7 +4259,7 @@
       </c>
     </row>
     <row r="53" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="55"/>
+      <c r="A53" s="59"/>
       <c r="B53" s="14" t="s">
         <v>47</v>
       </c>
@@ -4276,7 +4284,7 @@
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="55"/>
+      <c r="A54" s="59"/>
       <c r="B54" s="13"/>
       <c r="C54" s="35"/>
       <c r="F54" s="24"/>
@@ -4285,7 +4293,7 @@
       </c>
     </row>
     <row r="55" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A55" s="55"/>
+      <c r="A55" s="59"/>
       <c r="B55" s="13"/>
       <c r="C55" s="35"/>
       <c r="F55" s="24"/>
@@ -4312,7 +4320,7 @@
       </c>
     </row>
     <row r="56" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A56" s="55"/>
+      <c r="A56" s="59"/>
       <c r="B56" s="13"/>
       <c r="C56" s="35"/>
       <c r="F56" s="24"/>
@@ -4321,7 +4329,7 @@
       </c>
     </row>
     <row r="57" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="55"/>
+      <c r="A57" s="59"/>
       <c r="B57" s="13"/>
       <c r="C57" s="35"/>
       <c r="F57" s="24"/>
@@ -4332,7 +4340,7 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="55"/>
+      <c r="A58" s="59"/>
       <c r="B58" s="13"/>
       <c r="C58" s="35"/>
       <c r="F58" s="24"/>
@@ -4341,7 +4349,7 @@
       </c>
     </row>
     <row r="59" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A59" s="55"/>
+      <c r="A59" s="59"/>
       <c r="B59" s="13"/>
       <c r="C59" s="35"/>
       <c r="F59" s="24"/>
@@ -4368,7 +4376,7 @@
       </c>
     </row>
     <row r="60" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A60" s="55"/>
+      <c r="A60" s="59"/>
       <c r="B60" s="13"/>
       <c r="C60" s="35"/>
       <c r="F60" s="24"/>
@@ -4377,7 +4385,7 @@
       </c>
     </row>
     <row r="61" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A61" s="55"/>
+      <c r="A61" s="59"/>
       <c r="B61" s="13"/>
       <c r="C61" s="35"/>
       <c r="F61" s="24"/>
@@ -4388,7 +4396,7 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" s="55"/>
+      <c r="A62" s="59"/>
       <c r="B62" s="13"/>
       <c r="C62" s="35"/>
       <c r="F62" s="24"/>
@@ -4397,7 +4405,7 @@
       </c>
     </row>
     <row r="63" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A63" s="55"/>
+      <c r="A63" s="59"/>
       <c r="B63" s="13"/>
       <c r="C63" s="35"/>
       <c r="F63" s="24"/>
@@ -4422,7 +4430,7 @@
       </c>
     </row>
     <row r="64" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A64" s="55"/>
+      <c r="A64" s="59"/>
       <c r="B64" s="13"/>
       <c r="C64" s="35"/>
       <c r="F64" s="24"/>
@@ -4431,7 +4439,7 @@
       </c>
     </row>
     <row r="65" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A65" s="55"/>
+      <c r="A65" s="59"/>
       <c r="B65" s="13"/>
       <c r="C65" s="35"/>
       <c r="F65" s="24"/>
@@ -4442,7 +4450,7 @@
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="55"/>
+      <c r="A66" s="59"/>
       <c r="B66" s="13"/>
       <c r="C66" s="35"/>
       <c r="F66" s="24"/>
@@ -4451,7 +4459,7 @@
       </c>
     </row>
     <row r="67" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A67" s="55"/>
+      <c r="A67" s="59"/>
       <c r="B67" s="13"/>
       <c r="C67" s="35"/>
       <c r="F67" s="24"/>
@@ -4476,7 +4484,7 @@
       </c>
     </row>
     <row r="68" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A68" s="55"/>
+      <c r="A68" s="59"/>
       <c r="B68" s="13"/>
       <c r="C68" s="35"/>
       <c r="F68" s="24"/>
@@ -4485,7 +4493,7 @@
       </c>
     </row>
     <row r="69" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="55"/>
+      <c r="A69" s="59"/>
       <c r="B69" s="13"/>
       <c r="C69" s="35"/>
       <c r="F69" s="24"/>
@@ -4496,7 +4504,7 @@
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="56" t="s">
+      <c r="A70" s="60" t="s">
         <v>48</v>
       </c>
       <c r="B70" s="11" t="s">
@@ -4519,7 +4527,7 @@
       </c>
     </row>
     <row r="71" spans="1:7" ht="180" x14ac:dyDescent="0.25">
-      <c r="A71" s="56"/>
+      <c r="A71" s="60"/>
       <c r="B71" s="12" t="s">
         <v>50</v>
       </c>
@@ -4561,7 +4569,7 @@
       </c>
     </row>
     <row r="72" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A72" s="56"/>
+      <c r="A72" s="60"/>
       <c r="B72" s="13" t="s">
         <v>51</v>
       </c>
@@ -4582,7 +4590,7 @@
       </c>
     </row>
     <row r="73" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A73" s="56"/>
+      <c r="A73" s="60"/>
       <c r="B73" s="14" t="s">
         <v>47</v>
       </c>
@@ -4603,7 +4611,7 @@
       </c>
     </row>
     <row r="74" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A74" s="56"/>
+      <c r="A74" s="60"/>
       <c r="B74" s="13" t="s">
         <v>52</v>
       </c>
@@ -4622,7 +4630,7 @@
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A75" s="55" t="s">
+      <c r="A75" s="59" t="s">
         <v>53</v>
       </c>
       <c r="B75" s="7" t="s">
@@ -4650,7 +4658,7 @@
       </c>
     </row>
     <row r="76" spans="1:7" ht="240" x14ac:dyDescent="0.25">
-      <c r="A76" s="56"/>
+      <c r="A76" s="60"/>
       <c r="B76" s="8" t="s">
         <v>55</v>
       </c>
@@ -4739,7 +4747,7 @@
       </c>
     </row>
     <row r="77" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A77" s="56"/>
+      <c r="A77" s="60"/>
       <c r="B77" s="8" t="s">
         <v>56</v>
       </c>
@@ -4760,7 +4768,7 @@
       </c>
     </row>
     <row r="78" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A78" s="56"/>
+      <c r="A78" s="60"/>
       <c r="B78" s="15" t="s">
         <v>57</v>
       </c>
@@ -4781,7 +4789,7 @@
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="55" t="s">
+      <c r="A79" s="59" t="s">
         <v>58</v>
       </c>
       <c r="B79" s="7" t="s">
@@ -4809,7 +4817,7 @@
       </c>
     </row>
     <row r="80" spans="1:7" ht="255" x14ac:dyDescent="0.25">
-      <c r="A80" s="55"/>
+      <c r="A80" s="59"/>
       <c r="B80" s="8" t="s">
         <v>60</v>
       </c>
@@ -4878,7 +4886,7 @@
       </c>
     </row>
     <row r="81" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A81" s="55"/>
+      <c r="A81" s="59"/>
       <c r="B81" s="8" t="s">
         <v>61</v>
       </c>
@@ -4907,7 +4915,7 @@
       </c>
     </row>
     <row r="82" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A82" s="55"/>
+      <c r="A82" s="59"/>
       <c r="B82" s="15" t="s">
         <v>47</v>
       </c>
@@ -4936,7 +4944,7 @@
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A83" s="55" t="s">
+      <c r="A83" s="59" t="s">
         <v>148</v>
       </c>
       <c r="B83" s="7" t="s">
@@ -4964,7 +4972,7 @@
       </c>
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A84" s="55"/>
+      <c r="A84" s="59"/>
       <c r="B84" s="8"/>
       <c r="C84" s="41" t="s">
         <v>94</v>
@@ -4983,7 +4991,7 @@
       </c>
     </row>
     <row r="85" spans="1:7" ht="225" x14ac:dyDescent="0.25">
-      <c r="A85" s="55"/>
+      <c r="A85" s="59"/>
       <c r="B85" s="8"/>
       <c r="C85" s="21" t="s">
         <v>187</v>
@@ -5038,7 +5046,7 @@
       </c>
     </row>
     <row r="86" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A86" s="55"/>
+      <c r="A86" s="59"/>
       <c r="B86" s="8"/>
       <c r="C86" s="25" t="str">
         <f ca="1">$C86</f>
@@ -5056,7 +5064,7 @@
       </c>
     </row>
     <row r="87" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A87" s="55"/>
+      <c r="A87" s="59"/>
       <c r="B87" s="8"/>
       <c r="C87" s="22" t="str">
         <f>$B15</f>
@@ -5080,7 +5088,7 @@
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A88" s="55"/>
+      <c r="A88" s="59"/>
       <c r="B88" s="8"/>
       <c r="C88" s="41" t="s">
         <v>174</v>
@@ -5093,7 +5101,7 @@
       </c>
     </row>
     <row r="89" spans="1:7" ht="240" x14ac:dyDescent="0.25">
-      <c r="A89" s="55"/>
+      <c r="A89" s="59"/>
       <c r="B89" s="8"/>
       <c r="C89" s="21" t="s">
         <v>188</v>
@@ -5138,7 +5146,7 @@
       </c>
     </row>
     <row r="90" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A90" s="55"/>
+      <c r="A90" s="59"/>
       <c r="B90" s="8"/>
       <c r="C90" s="25" t="str">
         <f ca="1">$C90</f>
@@ -5155,7 +5163,7 @@
       </c>
     </row>
     <row r="91" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A91" s="55"/>
+      <c r="A91" s="59"/>
       <c r="B91" s="8"/>
       <c r="C91" s="50" t="str">
         <f t="shared" ref="C91" si="0">$B35</f>
@@ -5174,7 +5182,7 @@
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A92" s="55"/>
+      <c r="A92" s="59"/>
       <c r="B92" s="8"/>
       <c r="C92" s="41" t="s">
         <v>95</v>
@@ -5184,7 +5192,7 @@
       </c>
     </row>
     <row r="93" spans="1:7" ht="240" x14ac:dyDescent="0.25">
-      <c r="A93" s="55"/>
+      <c r="A93" s="59"/>
       <c r="B93" s="8"/>
       <c r="C93" s="21" t="s">
         <v>164</v>
@@ -5210,7 +5218,7 @@
       </c>
     </row>
     <row r="94" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A94" s="55"/>
+      <c r="A94" s="59"/>
       <c r="B94" s="8"/>
       <c r="C94" s="25" t="str">
         <f ca="1">$C94</f>
@@ -5224,7 +5232,7 @@
       </c>
     </row>
     <row r="95" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A95" s="55"/>
+      <c r="A95" s="59"/>
       <c r="B95" s="8"/>
       <c r="C95" s="22" t="str">
         <f>$B15</f>
@@ -5238,7 +5246,7 @@
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A96" s="55"/>
+      <c r="A96" s="59"/>
       <c r="B96" s="8"/>
       <c r="C96" s="41" t="s">
         <v>96</v>
@@ -5248,7 +5256,7 @@
       </c>
     </row>
     <row r="97" spans="1:7" ht="255" x14ac:dyDescent="0.25">
-      <c r="A97" s="55"/>
+      <c r="A97" s="59"/>
       <c r="B97" s="8"/>
       <c r="C97" s="21" t="s">
         <v>165</v>
@@ -5274,7 +5282,7 @@
       </c>
     </row>
     <row r="98" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A98" s="55"/>
+      <c r="A98" s="59"/>
       <c r="B98" s="8"/>
       <c r="C98" s="25" t="str">
         <f ca="1">$C98</f>
@@ -5288,7 +5296,7 @@
       </c>
     </row>
     <row r="99" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A99" s="55"/>
+      <c r="A99" s="59"/>
       <c r="B99" s="8"/>
       <c r="C99" s="22" t="str">
         <f>$B19</f>
@@ -5302,7 +5310,7 @@
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A100" s="55"/>
+      <c r="A100" s="59"/>
       <c r="B100" s="8"/>
       <c r="C100" s="22"/>
       <c r="D100" s="41" t="s">
@@ -5310,7 +5318,7 @@
       </c>
     </row>
     <row r="101" spans="1:7" ht="165" x14ac:dyDescent="0.25">
-      <c r="A101" s="55"/>
+      <c r="A101" s="59"/>
       <c r="B101" s="8"/>
       <c r="C101" s="22"/>
       <c r="D101" s="21" t="str">
@@ -5334,7 +5342,7 @@
       </c>
     </row>
     <row r="102" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A102" s="55"/>
+      <c r="A102" s="59"/>
       <c r="B102" s="8"/>
       <c r="C102" s="22"/>
       <c r="D102" s="25" t="str">
@@ -5344,7 +5352,7 @@
       </c>
     </row>
     <row r="103" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A103" s="55"/>
+      <c r="A103" s="59"/>
       <c r="B103" s="8"/>
       <c r="C103" s="22"/>
       <c r="D103" s="22" t="str">
@@ -5354,7 +5362,7 @@
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A104" s="55" t="s">
+      <c r="A104" s="59" t="s">
         <v>63</v>
       </c>
       <c r="B104" s="7" t="s">
@@ -5382,7 +5390,7 @@
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A105" s="55"/>
+      <c r="A105" s="59"/>
       <c r="B105" s="8"/>
       <c r="C105" s="41" t="s">
         <v>172</v>
@@ -5399,7 +5407,7 @@
       <c r="G105" s="41"/>
     </row>
     <row r="106" spans="1:7" ht="303" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="56"/>
+      <c r="A106" s="60"/>
       <c r="B106" s="8" t="s">
         <v>65</v>
       </c>
@@ -5420,7 +5428,7 @@
       </c>
     </row>
     <row r="107" spans="1:7" ht="84" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="56"/>
+      <c r="A107" s="60"/>
       <c r="B107" s="8" t="s">
         <v>66</v>
       </c>
@@ -5439,7 +5447,7 @@
       <c r="G107" s="25"/>
     </row>
     <row r="108" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A108" s="56"/>
+      <c r="A108" s="60"/>
       <c r="B108" s="8" t="s">
         <v>47</v>
       </c>
@@ -5458,7 +5466,7 @@
       <c r="G108" s="22"/>
     </row>
     <row r="109" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A109" s="59"/>
+      <c r="A109" s="55"/>
       <c r="B109" s="13" t="s">
         <v>52</v>
       </c>
@@ -5474,7 +5482,7 @@
       <c r="G109" s="24"/>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A110" s="55"/>
+      <c r="A110" s="59"/>
       <c r="B110" s="8"/>
       <c r="C110" s="41" t="s">
         <v>97</v>
@@ -5489,7 +5497,7 @@
       <c r="G110" s="41"/>
     </row>
     <row r="111" spans="1:7" ht="250.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="56"/>
+      <c r="A111" s="60"/>
       <c r="B111" s="8" t="s">
         <v>65</v>
       </c>
@@ -5508,7 +5516,7 @@
       </c>
     </row>
     <row r="112" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A112" s="56"/>
+      <c r="A112" s="60"/>
       <c r="B112" s="8" t="s">
         <v>66</v>
       </c>
@@ -5525,7 +5533,7 @@
       <c r="G112" s="25"/>
     </row>
     <row r="113" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A113" s="56"/>
+      <c r="A113" s="60"/>
       <c r="B113" s="8" t="s">
         <v>47</v>
       </c>
@@ -5542,7 +5550,7 @@
       <c r="G113" s="22"/>
     </row>
     <row r="114" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A114" s="59"/>
+      <c r="A114" s="55"/>
       <c r="B114" s="13" t="s">
         <v>52</v>
       </c>
@@ -5556,7 +5564,7 @@
       <c r="G114" s="24"/>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A115" s="59"/>
+      <c r="A115" s="55"/>
       <c r="B115" s="8"/>
       <c r="C115" s="41" t="s">
         <v>173</v>
@@ -5566,7 +5574,7 @@
       </c>
     </row>
     <row r="116" spans="1:7" ht="225" x14ac:dyDescent="0.25">
-      <c r="A116" s="59"/>
+      <c r="A116" s="55"/>
       <c r="B116" s="8"/>
       <c r="C116" s="21" t="s">
         <v>180</v>
@@ -5576,7 +5584,7 @@
       </c>
     </row>
     <row r="117" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A117" s="59"/>
+      <c r="A117" s="55"/>
       <c r="B117" s="8"/>
       <c r="C117" s="25" t="s">
         <v>181</v>
@@ -5586,7 +5594,7 @@
       </c>
     </row>
     <row r="118" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A118" s="59"/>
+      <c r="A118" s="55"/>
       <c r="B118" s="8"/>
       <c r="C118" s="22" t="s">
         <v>171</v>
@@ -5596,7 +5604,7 @@
       </c>
     </row>
     <row r="119" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A119" s="59"/>
+      <c r="A119" s="55"/>
       <c r="B119" s="8"/>
       <c r="C119" s="24" t="s">
         <v>102</v>
@@ -5606,7 +5614,7 @@
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A120" s="59"/>
+      <c r="A120" s="55"/>
       <c r="B120" s="8"/>
       <c r="C120" s="41" t="s">
         <v>103</v>
@@ -5616,7 +5624,7 @@
       </c>
     </row>
     <row r="121" spans="1:7" ht="240" x14ac:dyDescent="0.25">
-      <c r="A121" s="59"/>
+      <c r="A121" s="55"/>
       <c r="B121" s="8"/>
       <c r="C121" s="21" t="s">
         <v>179</v>
@@ -5626,7 +5634,7 @@
       </c>
     </row>
     <row r="122" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A122" s="59"/>
+      <c r="A122" s="55"/>
       <c r="B122" s="8"/>
       <c r="C122" s="25" t="s">
         <v>104</v>
@@ -5636,7 +5644,7 @@
       </c>
     </row>
     <row r="123" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A123" s="59"/>
+      <c r="A123" s="55"/>
       <c r="B123" s="8"/>
       <c r="C123" s="22" t="s">
         <v>105</v>
@@ -5646,7 +5654,7 @@
       </c>
     </row>
     <row r="124" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A124" s="59"/>
+      <c r="A124" s="55"/>
       <c r="B124" s="8"/>
       <c r="C124" s="24" t="s">
         <v>102</v>
@@ -5656,42 +5664,42 @@
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A125" s="59"/>
+      <c r="A125" s="55"/>
       <c r="B125" s="8"/>
       <c r="C125" s="41" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="126" spans="1:7" ht="240" x14ac:dyDescent="0.25">
-      <c r="A126" s="59"/>
+      <c r="A126" s="55"/>
       <c r="B126" s="8"/>
       <c r="C126" s="21" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="127" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A127" s="59"/>
+      <c r="A127" s="55"/>
       <c r="B127" s="8"/>
       <c r="C127" s="25" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="128" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A128" s="59"/>
+      <c r="A128" s="55"/>
       <c r="B128" s="8"/>
       <c r="C128" s="22" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="129" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A129" s="59"/>
+      <c r="A129" s="55"/>
       <c r="B129" s="8"/>
       <c r="C129" s="24" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A130" s="55" t="s">
+      <c r="A130" s="59" t="s">
         <v>67</v>
       </c>
       <c r="B130" s="7" t="s">
@@ -5714,7 +5722,7 @@
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A131" s="55"/>
+      <c r="A131" s="59"/>
       <c r="B131" s="12"/>
       <c r="C131" s="42" t="s">
         <v>109</v>
@@ -5730,7 +5738,7 @@
       </c>
     </row>
     <row r="132" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A132" s="56"/>
+      <c r="A132" s="60"/>
       <c r="B132" s="8" t="s">
         <v>69</v>
       </c>
@@ -5752,7 +5760,7 @@
       </c>
     </row>
     <row r="133" spans="1:7" ht="330" x14ac:dyDescent="0.25">
-      <c r="A133" s="56"/>
+      <c r="A133" s="60"/>
       <c r="B133" s="8" t="s">
         <v>216</v>
       </c>
@@ -5770,7 +5778,7 @@
       </c>
     </row>
     <row r="134" spans="1:7" ht="165" x14ac:dyDescent="0.25">
-      <c r="A134" s="56"/>
+      <c r="A134" s="60"/>
       <c r="B134" s="8" t="s">
         <v>208</v>
       </c>
@@ -5787,17 +5795,15 @@
         <v>90</v>
       </c>
     </row>
-    <row r="135" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A135" s="56"/>
+    <row r="135" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A135" s="60"/>
       <c r="B135" s="5" t="str">
         <f>$B7</f>
         <v>#### Clearing:
 - not applicable</v>
       </c>
-      <c r="C135" s="45" t="str">
-        <f>$B7</f>
-        <v>#### Clearing:
-- not applicable</v>
+      <c r="C135" s="45" t="s">
+        <v>227</v>
       </c>
       <c r="D135" s="45" t="str">
         <f>$B7</f>
@@ -5812,7 +5818,7 @@
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A136" s="55" t="s">
+      <c r="A136" s="59" t="s">
         <v>70</v>
       </c>
       <c r="B136" s="11" t="s">
@@ -5835,7 +5841,7 @@
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A137" s="55"/>
+      <c r="A137" s="59"/>
       <c r="B137" s="13"/>
       <c r="C137" s="39" t="s">
         <v>90</v>
@@ -5851,7 +5857,7 @@
       </c>
     </row>
     <row r="138" spans="1:7" ht="237.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A138" s="55"/>
+      <c r="A138" s="59"/>
       <c r="B138" s="12" t="s">
         <v>72</v>
       </c>
@@ -5869,7 +5875,7 @@
       </c>
     </row>
     <row r="139" spans="1:7" ht="105" x14ac:dyDescent="0.25">
-      <c r="A139" s="55"/>
+      <c r="A139" s="59"/>
       <c r="B139" s="13" t="s">
         <v>73</v>
       </c>
@@ -5887,7 +5893,7 @@
       </c>
     </row>
     <row r="140" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A140" s="55"/>
+      <c r="A140" s="59"/>
       <c r="B140" s="13" t="s">
         <v>47</v>
       </c>
@@ -5900,7 +5906,7 @@
       </c>
     </row>
     <row r="141" spans="1:7" ht="60" x14ac:dyDescent="0.25">
-      <c r="A141" s="55"/>
+      <c r="A141" s="59"/>
       <c r="B141" s="13" t="s">
         <v>52</v>
       </c>
@@ -5913,7 +5919,7 @@
       </c>
     </row>
     <row r="142" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A142" s="55" t="s">
+      <c r="A142" s="59" t="s">
         <v>74</v>
       </c>
       <c r="B142" s="7" t="s">
@@ -5936,7 +5942,7 @@
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A143" s="55"/>
+      <c r="A143" s="59"/>
       <c r="B143" s="8"/>
       <c r="C143" s="41" t="s">
         <v>169</v>
@@ -5952,7 +5958,7 @@
       </c>
     </row>
     <row r="144" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A144" s="55"/>
+      <c r="A144" s="59"/>
       <c r="B144" s="8" t="s">
         <v>41</v>
       </c>
@@ -5970,7 +5976,7 @@
       </c>
     </row>
     <row r="145" spans="1:6" ht="388.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A145" s="55"/>
+      <c r="A145" s="59"/>
       <c r="B145" s="8" t="s">
         <v>210</v>
       </c>
@@ -5988,7 +5994,7 @@
       </c>
     </row>
     <row r="146" spans="1:6" ht="150" x14ac:dyDescent="0.25">
-      <c r="A146" s="55"/>
+      <c r="A146" s="59"/>
       <c r="B146" s="8" t="s">
         <v>212</v>
       </c>
@@ -6000,7 +6006,7 @@
       </c>
     </row>
     <row r="147" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A147" s="55"/>
+      <c r="A147" s="59"/>
       <c r="B147" s="8" t="s">
         <v>47</v>
       </c>
@@ -6012,7 +6018,7 @@
       </c>
     </row>
     <row r="148" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A148" s="55"/>
+      <c r="A148" s="59"/>
       <c r="B148" s="13" t="s">
         <v>52</v>
       </c>
@@ -6024,7 +6030,7 @@
       </c>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A149" s="55"/>
+      <c r="A149" s="59"/>
       <c r="B149" s="8"/>
       <c r="C149" s="41" t="s">
         <v>112</v>
@@ -6040,7 +6046,7 @@
       </c>
     </row>
     <row r="150" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A150" s="55"/>
+      <c r="A150" s="59"/>
       <c r="B150" s="8" t="s">
         <v>41</v>
       </c>
@@ -6058,7 +6064,7 @@
       </c>
     </row>
     <row r="151" spans="1:6" ht="345" x14ac:dyDescent="0.25">
-      <c r="A151" s="55"/>
+      <c r="A151" s="59"/>
       <c r="B151" s="8" t="s">
         <v>210</v>
       </c>
@@ -6076,7 +6082,7 @@
       </c>
     </row>
     <row r="152" spans="1:6" ht="150" x14ac:dyDescent="0.25">
-      <c r="A152" s="55"/>
+      <c r="A152" s="59"/>
       <c r="B152" s="8" t="s">
         <v>212</v>
       </c>
@@ -6088,7 +6094,7 @@
       </c>
     </row>
     <row r="153" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A153" s="55"/>
+      <c r="A153" s="59"/>
       <c r="B153" s="8" t="s">
         <v>47</v>
       </c>
@@ -6100,7 +6106,7 @@
       </c>
     </row>
     <row r="154" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A154" s="55"/>
+      <c r="A154" s="59"/>
       <c r="B154" s="13" t="s">
         <v>52</v>
       </c>
@@ -6112,7 +6118,7 @@
       </c>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A155" s="55"/>
+      <c r="A155" s="59"/>
       <c r="B155" s="8"/>
       <c r="C155" s="41" t="s">
         <v>168</v>
@@ -6122,7 +6128,7 @@
       </c>
     </row>
     <row r="156" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A156" s="55"/>
+      <c r="A156" s="59"/>
       <c r="B156" s="8"/>
       <c r="C156" s="31" t="s">
         <v>41</v>
@@ -6132,7 +6138,7 @@
       </c>
     </row>
     <row r="157" spans="1:6" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A157" s="55"/>
+      <c r="A157" s="59"/>
       <c r="B157" s="8"/>
       <c r="C157" s="21" t="s">
         <v>214</v>
@@ -6142,7 +6148,7 @@
       </c>
     </row>
     <row r="158" spans="1:6" ht="135" x14ac:dyDescent="0.25">
-      <c r="A158" s="55"/>
+      <c r="A158" s="59"/>
       <c r="B158" s="8"/>
       <c r="C158" s="29" t="s">
         <v>219</v>
@@ -6152,7 +6158,7 @@
       </c>
     </row>
     <row r="159" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A159" s="55"/>
+      <c r="A159" s="59"/>
       <c r="B159" s="8"/>
       <c r="C159" s="22" t="s">
         <v>171</v>
@@ -6162,7 +6168,7 @@
       </c>
     </row>
     <row r="160" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="A160" s="55"/>
+      <c r="A160" s="59"/>
       <c r="B160" s="8"/>
       <c r="C160" s="24" t="s">
         <v>102</v>
@@ -6172,7 +6178,7 @@
       </c>
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A161" s="55"/>
+      <c r="A161" s="59"/>
       <c r="B161" s="8"/>
       <c r="C161" s="41" t="s">
         <v>114</v>
@@ -6182,7 +6188,7 @@
       </c>
     </row>
     <row r="162" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A162" s="55"/>
+      <c r="A162" s="59"/>
       <c r="B162" s="8"/>
       <c r="C162" s="31" t="s">
         <v>41</v>
@@ -6192,7 +6198,7 @@
       </c>
     </row>
     <row r="163" spans="1:7" ht="360" x14ac:dyDescent="0.25">
-      <c r="A163" s="55"/>
+      <c r="A163" s="59"/>
       <c r="B163" s="8"/>
       <c r="C163" s="21" t="s">
         <v>197</v>
@@ -6202,7 +6208,7 @@
       </c>
     </row>
     <row r="164" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A164" s="55"/>
+      <c r="A164" s="59"/>
       <c r="B164" s="8"/>
       <c r="C164" s="29" t="s">
         <v>219</v>
@@ -6212,7 +6218,7 @@
       </c>
     </row>
     <row r="165" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A165" s="55"/>
+      <c r="A165" s="59"/>
       <c r="B165" s="8"/>
       <c r="C165" s="22" t="s">
         <v>105</v>
@@ -6222,7 +6228,7 @@
       </c>
     </row>
     <row r="166" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A166" s="55"/>
+      <c r="A166" s="59"/>
       <c r="B166" s="8"/>
       <c r="C166" s="24" t="s">
         <v>102</v>
@@ -6232,49 +6238,49 @@
       </c>
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A167" s="55"/>
+      <c r="A167" s="59"/>
       <c r="B167" s="8"/>
       <c r="C167" s="41" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="168" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A168" s="55"/>
+      <c r="A168" s="59"/>
       <c r="B168" s="8"/>
       <c r="C168" s="31" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="169" spans="1:7" ht="360" x14ac:dyDescent="0.25">
-      <c r="A169" s="55"/>
+      <c r="A169" s="59"/>
       <c r="B169" s="8"/>
       <c r="C169" s="21" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="170" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A170" s="55"/>
+      <c r="A170" s="59"/>
       <c r="B170" s="8"/>
       <c r="C170" s="29" t="s">
         <v>219</v>
       </c>
     </row>
     <row r="171" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A171" s="55"/>
+      <c r="A171" s="59"/>
       <c r="B171" s="8"/>
       <c r="C171" s="22" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="172" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A172" s="55"/>
+      <c r="A172" s="59"/>
       <c r="B172" s="8"/>
       <c r="C172" s="24" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="173" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A173" s="56" t="s">
+      <c r="A173" s="60" t="s">
         <v>76</v>
       </c>
       <c r="B173" s="7" t="s">
@@ -6297,7 +6303,7 @@
       </c>
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A174" s="56"/>
+      <c r="A174" s="60"/>
       <c r="B174" s="8"/>
       <c r="C174" s="31" t="s">
         <v>90</v>
@@ -6313,7 +6319,7 @@
       </c>
     </row>
     <row r="175" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A175" s="56"/>
+      <c r="A175" s="60"/>
       <c r="B175" s="8" t="s">
         <v>41</v>
       </c>
@@ -6331,7 +6337,7 @@
       </c>
     </row>
     <row r="176" spans="1:7" ht="332.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A176" s="56"/>
+      <c r="A176" s="60"/>
       <c r="B176" s="8" t="s">
         <v>200</v>
       </c>
@@ -6349,7 +6355,7 @@
       </c>
     </row>
     <row r="177" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A177" s="56"/>
+      <c r="A177" s="60"/>
       <c r="B177" s="8" t="s">
         <v>201</v>
       </c>
@@ -6359,7 +6365,7 @@
       </c>
     </row>
     <row r="178" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A178" s="56"/>
+      <c r="A178" s="60"/>
       <c r="B178" s="15" t="s">
         <v>47</v>
       </c>
@@ -6369,7 +6375,7 @@
       </c>
     </row>
     <row r="179" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A179" s="56"/>
+      <c r="A179" s="60"/>
       <c r="B179" s="13" t="s">
         <v>52</v>
       </c>
@@ -6379,7 +6385,7 @@
       </c>
     </row>
     <row r="180" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A180" s="56" t="s">
+      <c r="A180" s="60" t="s">
         <v>78</v>
       </c>
       <c r="B180" s="7" t="s">
@@ -6402,7 +6408,7 @@
       </c>
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A181" s="56"/>
+      <c r="A181" s="60"/>
       <c r="B181" s="8"/>
       <c r="C181" s="46"/>
       <c r="D181" s="41" t="s">
@@ -6412,7 +6418,7 @@
       <c r="F181" s="46"/>
     </row>
     <row r="182" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A182" s="56"/>
+      <c r="A182" s="60"/>
       <c r="B182" s="8" t="s">
         <v>41</v>
       </c>
@@ -6429,8 +6435,8 @@
         <v>90</v>
       </c>
     </row>
-    <row r="183" spans="1:7" ht="255" x14ac:dyDescent="0.25">
-      <c r="A183" s="56"/>
+    <row r="183" spans="1:7" ht="240" x14ac:dyDescent="0.25">
+      <c r="A183" s="60"/>
       <c r="B183" s="8" t="s">
         <v>200</v>
       </c>
@@ -6448,7 +6454,7 @@
       </c>
     </row>
     <row r="184" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A184" s="56"/>
+      <c r="A184" s="60"/>
       <c r="B184" s="8" t="s">
         <v>202</v>
       </c>
@@ -6458,7 +6464,7 @@
       </c>
     </row>
     <row r="185" spans="1:7" ht="45" x14ac:dyDescent="0.25">
-      <c r="A185" s="56"/>
+      <c r="A185" s="60"/>
       <c r="B185" s="15" t="s">
         <v>47</v>
       </c>
@@ -6468,7 +6474,7 @@
       </c>
     </row>
     <row r="186" spans="1:7" ht="75" x14ac:dyDescent="0.25">
-      <c r="A186" s="56"/>
+      <c r="A186" s="60"/>
       <c r="B186" s="13" t="s">
         <v>52</v>
       </c>
@@ -6478,7 +6484,7 @@
       </c>
     </row>
     <row r="187" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A187" s="56" t="s">
+      <c r="A187" s="60" t="s">
         <v>80</v>
       </c>
       <c r="B187" s="7" t="s">
@@ -6501,7 +6507,7 @@
       </c>
     </row>
     <row r="188" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A188" s="56"/>
+      <c r="A188" s="60"/>
       <c r="B188" s="8" t="s">
         <v>41</v>
       </c>
@@ -6519,7 +6525,7 @@
       </c>
     </row>
     <row r="189" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A189" s="56"/>
+      <c r="A189" s="60"/>
       <c r="B189" s="8" t="s">
         <v>200</v>
       </c>
@@ -6537,28 +6543,28 @@
       </c>
     </row>
     <row r="190" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A190" s="56"/>
+      <c r="A190" s="60"/>
       <c r="B190" s="8" t="s">
         <v>203</v>
       </c>
       <c r="C190" s="29"/>
     </row>
     <row r="191" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A191" s="56"/>
+      <c r="A191" s="60"/>
       <c r="B191" s="15" t="s">
         <v>47</v>
       </c>
       <c r="C191" s="29"/>
     </row>
     <row r="192" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A192" s="59"/>
+      <c r="A192" s="55"/>
       <c r="B192" s="13" t="s">
         <v>52</v>
       </c>
       <c r="C192" s="29"/>
     </row>
     <row r="193" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A193" s="56" t="s">
+      <c r="A193" s="60" t="s">
         <v>82</v>
       </c>
       <c r="B193" s="7" t="s">
@@ -6581,7 +6587,7 @@
       </c>
     </row>
     <row r="194" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A194" s="56"/>
+      <c r="A194" s="60"/>
       <c r="B194" s="8" t="s">
         <v>41</v>
       </c>
@@ -6599,7 +6605,7 @@
       </c>
     </row>
     <row r="195" spans="1:7" ht="135" x14ac:dyDescent="0.25">
-      <c r="A195" s="56"/>
+      <c r="A195" s="60"/>
       <c r="B195" s="8" t="s">
         <v>200</v>
       </c>
@@ -6617,13 +6623,13 @@
       </c>
     </row>
     <row r="196" spans="1:7" ht="150" x14ac:dyDescent="0.25">
-      <c r="A196" s="56"/>
+      <c r="A196" s="60"/>
       <c r="B196" s="8" t="s">
         <v>204</v>
       </c>
     </row>
     <row r="197" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A197" s="56"/>
+      <c r="A197" s="60"/>
       <c r="B197" s="8" t="s">
         <v>47</v>
       </c>
@@ -6632,7 +6638,7 @@
       </c>
     </row>
     <row r="198" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A198" s="56"/>
+      <c r="A198" s="60"/>
       <c r="B198" s="16" t="s">
         <v>52</v>
       </c>
@@ -6641,132 +6647,142 @@
       </c>
     </row>
     <row r="199" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A199" s="56"/>
+      <c r="A199" s="60"/>
       <c r="C199" s="29"/>
     </row>
     <row r="200" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A200" s="60"/>
+      <c r="A200" s="57"/>
       <c r="C200" s="49"/>
     </row>
     <row r="201" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A201" s="60"/>
+      <c r="A201" s="57"/>
     </row>
     <row r="202" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A202" s="60"/>
+      <c r="A202" s="57"/>
     </row>
     <row r="203" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A203" s="60"/>
+      <c r="A203" s="57"/>
     </row>
     <row r="204" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A204" s="60"/>
+      <c r="A204" s="57"/>
     </row>
     <row r="205" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A205" s="60"/>
+      <c r="A205" s="57"/>
     </row>
     <row r="206" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A206" s="60"/>
+      <c r="A206" s="57"/>
     </row>
     <row r="207" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A207" s="60"/>
+      <c r="A207" s="57"/>
     </row>
     <row r="208" spans="1:7" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A208" s="60"/>
+      <c r="A208" s="57"/>
     </row>
     <row r="209" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A209" s="60"/>
+      <c r="A209" s="57"/>
     </row>
     <row r="210" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A210" s="60"/>
+      <c r="A210" s="57"/>
     </row>
     <row r="211" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A211" s="60"/>
+      <c r="A211" s="57"/>
     </row>
     <row r="212" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A212" s="60"/>
+      <c r="A212" s="57"/>
     </row>
     <row r="213" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A213" s="60"/>
+      <c r="A213" s="57"/>
     </row>
     <row r="214" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A214" s="60"/>
+      <c r="A214" s="57"/>
     </row>
     <row r="215" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A215" s="60"/>
+      <c r="A215" s="57"/>
     </row>
     <row r="216" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A216" s="60"/>
+      <c r="A216" s="57"/>
     </row>
     <row r="217" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A217" s="60"/>
+      <c r="A217" s="57"/>
     </row>
     <row r="218" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A218" s="60"/>
+      <c r="A218" s="57"/>
     </row>
     <row r="219" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A219" s="60"/>
+      <c r="A219" s="57"/>
     </row>
     <row r="220" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A220" s="60"/>
+      <c r="A220" s="57"/>
     </row>
     <row r="221" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A221" s="60"/>
+      <c r="A221" s="57"/>
     </row>
     <row r="222" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A222" s="60"/>
+      <c r="A222" s="57"/>
     </row>
     <row r="223" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A223" s="60"/>
+      <c r="A223" s="57"/>
     </row>
     <row r="224" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A224" s="60"/>
+      <c r="A224" s="57"/>
     </row>
     <row r="225" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A225" s="60"/>
+      <c r="A225" s="57"/>
     </row>
     <row r="226" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A226" s="60"/>
+      <c r="A226" s="57"/>
     </row>
     <row r="227" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A227" s="60"/>
+      <c r="A227" s="57"/>
     </row>
     <row r="228" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A228" s="60"/>
+      <c r="A228" s="57"/>
     </row>
     <row r="229" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A229" s="60"/>
+      <c r="A229" s="57"/>
     </row>
     <row r="230" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A230" s="60"/>
+      <c r="A230" s="57"/>
     </row>
     <row r="231" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A231" s="60"/>
+      <c r="A231" s="57"/>
     </row>
     <row r="232" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A232" s="60"/>
+      <c r="A232" s="57"/>
     </row>
     <row r="233" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A233" s="60"/>
+      <c r="A233" s="57"/>
     </row>
     <row r="234" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A234" s="60"/>
+      <c r="A234" s="57"/>
     </row>
     <row r="235" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A235" s="60"/>
+      <c r="A235" s="57"/>
     </row>
     <row r="236" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A236" s="60"/>
+      <c r="A236" s="57"/>
     </row>
     <row r="237" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A237" s="60"/>
+      <c r="A237" s="57"/>
     </row>
     <row r="238" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A238" s="60"/>
+      <c r="A238" s="57"/>
     </row>
     <row r="239" spans="1:1" s="53" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A239" s="60"/>
+      <c r="A239" s="57"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A4:A7"/>
+    <mergeCell ref="A8:A11"/>
+    <mergeCell ref="A12:A15"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A23"/>
+    <mergeCell ref="A24:A27"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="A32:A35"/>
+    <mergeCell ref="A36:A39"/>
+    <mergeCell ref="A40:A43"/>
     <mergeCell ref="A44:A48"/>
     <mergeCell ref="A193:A199"/>
     <mergeCell ref="A75:A78"/>
@@ -6782,16 +6798,6 @@
     <mergeCell ref="A180:A186"/>
     <mergeCell ref="A50:A69"/>
     <mergeCell ref="A70:A74"/>
-    <mergeCell ref="A24:A27"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="A32:A35"/>
-    <mergeCell ref="A36:A39"/>
-    <mergeCell ref="A40:A43"/>
-    <mergeCell ref="A4:A7"/>
-    <mergeCell ref="A8:A11"/>
-    <mergeCell ref="A12:A15"/>
-    <mergeCell ref="A16:A19"/>
-    <mergeCell ref="A20:A23"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>

</xml_diff>